<commit_message>
Try getting column header from index
</commit_message>
<xml_diff>
--- a/untitled.xlsx
+++ b/untitled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\World\Documents\SeniorProject\datast\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B432BA68-D2F8-458E-96E3-78A71C5276C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98447B00-25C8-400E-BC5E-090ED5EB2D11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ปี</t>
   </si>
@@ -42,112 +42,19 @@
     <t>พลังความร้อนร่วม</t>
   </si>
   <si>
-    <t>ดีเซล</t>
-  </si>
-  <si>
     <t>พลังงานทดแทน</t>
   </si>
   <si>
-    <t>อื่น ๆ</t>
-  </si>
-  <si>
-    <t>ซื้อ</t>
-  </si>
-  <si>
     <t>2559 </t>
   </si>
   <si>
-    <t>261.06  </t>
-  </si>
-  <si>
-    <t>0.09  </t>
-  </si>
-  <si>
-    <t>7.54  </t>
-  </si>
-  <si>
     <t>2560 </t>
   </si>
   <si>
-    <t>218.47  </t>
-  </si>
-  <si>
-    <t>0.35  </t>
-  </si>
-  <si>
-    <t>13.07  </t>
-  </si>
-  <si>
     <t>2561 </t>
   </si>
   <si>
-    <t>80.06  </t>
-  </si>
-  <si>
-    <t>0.10  </t>
-  </si>
-  <si>
-    <t>10.62  </t>
-  </si>
-  <si>
     <t>2562 </t>
-  </si>
-  <si>
-    <t>0.31  </t>
-  </si>
-  <si>
-    <t>0.13  </t>
-  </si>
-  <si>
-    <t>71.22  </t>
-  </si>
-  <si>
-    <t>20296.86  </t>
-  </si>
-  <si>
-    <t>17615.38  </t>
-  </si>
-  <si>
-    <t>16062.72  </t>
-  </si>
-  <si>
-    <t>17752.69  </t>
-  </si>
-  <si>
-    <t>3521.01  </t>
-  </si>
-  <si>
-    <t>4685.96  </t>
-  </si>
-  <si>
-    <t>7560.13  </t>
-  </si>
-  <si>
-    <t>6282.77  </t>
-  </si>
-  <si>
-    <t>43679.36  </t>
-  </si>
-  <si>
-    <t>38290.08  </t>
-  </si>
-  <si>
-    <t>37801.47  </t>
-  </si>
-  <si>
-    <t>38209.28  </t>
-  </si>
-  <si>
-    <t>121233.72  </t>
-  </si>
-  <si>
-    <t>128111.66  </t>
-  </si>
-  <si>
-    <t>129862.63  </t>
-  </si>
-  <si>
-    <t>135556.60  </t>
   </si>
 </sst>
 </file>
@@ -229,8 +136,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Comma 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -522,22 +432,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="2" max="2" width="11.265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -556,118 +466,85 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B2">
+        <v>20296.86</v>
+      </c>
+      <c r="C2" s="1">
+        <v>3521.01</v>
+      </c>
+      <c r="D2">
+        <v>261.06</v>
+      </c>
+      <c r="E2">
+        <v>43679.360000000001</v>
+      </c>
+      <c r="F2">
+        <v>43679.360000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="B3">
+        <v>17615.38</v>
+      </c>
+      <c r="C3">
+        <v>4685.96</v>
+      </c>
+      <c r="D3">
+        <v>218.47</v>
+      </c>
+      <c r="E3">
+        <v>38290.080000000002</v>
+      </c>
+      <c r="F3">
+        <v>37801.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
+      <c r="B4">
+        <v>16062.72</v>
+      </c>
+      <c r="C4">
+        <v>7560.13</v>
+      </c>
+      <c r="D4">
+        <v>80.06</v>
+      </c>
+      <c r="E4">
+        <v>37801.47</v>
+      </c>
+      <c r="F4">
+        <v>7560.13</v>
+      </c>
     </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
+      <c r="B5">
+        <v>17752.689999999999</v>
+      </c>
+      <c r="C5">
+        <v>6282.77</v>
+      </c>
+      <c r="D5">
+        <v>0.31</v>
+      </c>
+      <c r="E5">
+        <v>38209.279999999999</v>
+      </c>
+      <c r="F5">
+        <v>17752.689999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>